<commit_message>
temporary takedown of site
</commit_message>
<xml_diff>
--- a/data/timesheet.xlsx
+++ b/data/timesheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="7580" windowWidth="10440" windowHeight="10160" xr2:uid="{247C58A7-6264-3D4E-A960-D57B68684EDE}"/>
+    <workbookView xWindow="17020" yWindow="620" windowWidth="10440" windowHeight="10160" xr2:uid="{247C58A7-6264-3D4E-A960-D57B68684EDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BB605E-4798-DC4A-BA1D-6857BF56C83D}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,7 +534,15 @@
         <v>43140</v>
       </c>
       <c r="B11">
-        <v>1.5</v>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>43142</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -547,7 +555,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,7 +579,7 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -596,17 +604,17 @@
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Upgrade Python to 3.8; add zip+4 & ship to 48 states only
</commit_message>
<xml_diff>
--- a/data/timesheet.xlsx
+++ b/data/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wahhab/Sites/rts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C01C7F42-231A-9A42-B3D5-715B9ECD2BA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C2E9DB-A6C0-264C-8870-C2F6ACC2243F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24780" yWindow="13160" windowWidth="27640" windowHeight="16940" xr2:uid="{6BBACE2F-5368-244E-961E-2B2B095D7D80}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>TimeSheet for RTS Comics</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Review Spreadsheet Uploads</t>
+  </si>
+  <si>
+    <t>Access USPS data</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793FA332-5464-224F-832B-DC45C8D66E8E}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,6 +480,28 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43861</v>
+      </c>
+      <c r="B8">
+        <v>2.4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43862</v>
+      </c>
+      <c r="B9">
+        <v>1.9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update to Django 3.3.11, from email to donotreply
</commit_message>
<xml_diff>
--- a/data/timesheet.xlsx
+++ b/data/timesheet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wahhab/Sites/rts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C2E9DB-A6C0-264C-8870-C2F6ACC2243F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB8F152-647D-8346-96ED-5368E0D6DCDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24780" yWindow="13160" windowWidth="27640" windowHeight="16940" xr2:uid="{6BBACE2F-5368-244E-961E-2B2B095D7D80}"/>
+    <workbookView xWindow="24720" yWindow="13160" windowWidth="27640" windowHeight="16940" xr2:uid="{6BBACE2F-5368-244E-961E-2B2B095D7D80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>TimeSheet for RTS Comics</t>
   </si>
@@ -60,6 +60,24 @@
   </si>
   <si>
     <t>Access USPS data</t>
+  </si>
+  <si>
+    <t>Tried updating software versions</t>
+  </si>
+  <si>
+    <t>Head banging</t>
+  </si>
+  <si>
+    <t>Clean up, implement Z+4</t>
+  </si>
+  <si>
+    <t>Implement Zip+4, link to Ebay</t>
+  </si>
+  <si>
+    <t>More of same</t>
+  </si>
+  <si>
+    <t>Install update on pythoneverywhere</t>
   </si>
 </sst>
 </file>
@@ -412,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793FA332-5464-224F-832B-DC45C8D66E8E}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,6 +520,72 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43863</v>
+      </c>
+      <c r="B10">
+        <v>2.4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43864</v>
+      </c>
+      <c r="B11">
+        <v>2.5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43865</v>
+      </c>
+      <c r="B12">
+        <v>1.8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43865</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43866</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43875</v>
+      </c>
+      <c r="B15">
+        <v>1.4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>